<commit_message>
Updates BOM to link to correct acrylic sheet size and adds printed parts list.
</commit_message>
<xml_diff>
--- a/voron_2_tall_bom.xlsx
+++ b/voron_2_tall_bom.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ppak/GitHub/Voron-2-Tall/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A12C07A1-2F54-0944-A089-2D78562DA336}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBE1006C-2D86-C64B-B30D-9240C60A7B76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="7800" windowWidth="33600" windowHeight="21000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51200" yWindow="7800" windowWidth="33600" windowHeight="21000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="generated_bom" sheetId="1" r:id="rId1"/>
     <sheet name="custom_bom" sheetId="2" r:id="rId2"/>
+    <sheet name="custom_bom_white_orange" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="289">
   <si>
     <t>Category</t>
   </si>
@@ -874,6 +875,33 @@
   </si>
   <si>
     <t>Holes 10mm from each end</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B0C94YGTKX/ref=ox_sc_act_title_1?smid=A3E9XRLGZKR0KS&amp;th=1</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B0B5YJSQD3/ref=ewc_pr_img_2?smid=ATVPDKIKX0DER&amp;psc=1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rust-Oleum 372700 Acrylic Enamel 2X Spray Paint, 12 oz, Ultra Matte White </t>
+  </si>
+  <si>
+    <t>24" x 48" x 1/8" Orange</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B0C94XJYH7/ref=ewc_pr_img_1?smid=A3E9XRLGZKR0KS&amp;th=1</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/uxcell-Temperature-Multifunctional-Insulating-Transparent/dp/B0915QTF1G/ref=sr_1_5?crid=1TE27V508QIHN&amp;keywords=ptfe%2Btubing%2B1000mm%2B4mm%2BOD%2B3mm&amp;qid=1701900349&amp;s=industrial&amp;sprefix=ptfe%2Btubing%2B1000mm%2B4mm%2Bod%2B3mm%2Cindustrial%2C75&amp;sr=1-5&amp;th=1</t>
+  </si>
+  <si>
+    <t>9.84 ft</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/uxcell-Temperature-Multifunctional-Insulating-Transparent/dp/B0915BM1JD/ref=sr_1_5?crid=1TE27V508QIHN&amp;keywords=ptfe%2Btubing%2B1000mm%2B4mm%2BOD%2B3mm&amp;qid=1701900349&amp;s=industrial&amp;sprefix=ptfe%2Btubing%2B1000mm%2B4mm%2Bod%2B3mm%2Cindustrial%2C75&amp;sr=1-5&amp;th=1</t>
+  </si>
+  <si>
+    <t>36" x 24" x 1/8" Orange</t>
   </si>
 </sst>
 </file>
@@ -1442,7 +1470,87 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1855,8 +1963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L126"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="F79" sqref="F79"/>
+    <sheetView topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3208,7 +3316,7 @@
         <v>1</v>
       </c>
       <c r="F40" s="1">
-        <v>9.3000000000000007</v>
+        <v>13.8</v>
       </c>
       <c r="G40">
         <v>5</v>
@@ -3222,11 +3330,11 @@
       </c>
       <c r="J40" s="1">
         <f t="shared" si="4"/>
-        <v>46.5</v>
+        <v>69</v>
       </c>
       <c r="K40" s="1">
         <f t="shared" si="2"/>
-        <v>46.5</v>
+        <v>69</v>
       </c>
       <c r="L40" s="2" t="s">
         <v>145</v>
@@ -4933,7 +5041,16 @@
       <c r="C88">
         <v>1</v>
       </c>
+      <c r="D88" t="s">
+        <v>286</v>
+      </c>
       <c r="E88" t="b">
+        <v>1</v>
+      </c>
+      <c r="F88" s="1">
+        <v>7.99</v>
+      </c>
+      <c r="G88">
         <v>1</v>
       </c>
       <c r="H88">
@@ -4945,11 +5062,14 @@
       </c>
       <c r="J88" s="1">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>7.99</v>
       </c>
       <c r="K88" s="1">
         <f>(G88-H88)*F88</f>
-        <v>0</v>
+        <v>7.99</v>
+      </c>
+      <c r="L88" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.2">
@@ -4959,7 +5079,16 @@
       <c r="C89">
         <v>1</v>
       </c>
+      <c r="D89" t="s">
+        <v>286</v>
+      </c>
       <c r="E89" t="b">
+        <v>1</v>
+      </c>
+      <c r="F89" s="1">
+        <v>8.99</v>
+      </c>
+      <c r="G89">
         <v>1</v>
       </c>
       <c r="H89">
@@ -4971,11 +5100,14 @@
       </c>
       <c r="J89" s="1">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>8.99</v>
       </c>
       <c r="K89" s="1">
-        <f t="shared" ref="K89:K125" si="8">(G89-H89)*F89</f>
-        <v>0</v>
+        <f t="shared" ref="K89" si="8">(G89-H89)*F89</f>
+        <v>8.99</v>
+      </c>
+      <c r="L89" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.2">
@@ -5012,7 +5144,7 @@
         <v>0</v>
       </c>
       <c r="K90" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="K90:K125" si="9">(G90-H90)*F90</f>
         <v>11.99</v>
       </c>
       <c r="L90" t="s">
@@ -5047,7 +5179,7 @@
         <v>0</v>
       </c>
       <c r="K91" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>15.99</v>
       </c>
       <c r="L91" t="s">
@@ -5085,7 +5217,7 @@
         <v>0</v>
       </c>
       <c r="K92" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>15.49</v>
       </c>
       <c r="L92" t="s">
@@ -5123,7 +5255,7 @@
         <v>0</v>
       </c>
       <c r="K93" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>15.99</v>
       </c>
       <c r="L93" t="s">
@@ -5152,7 +5284,7 @@
         <v>0</v>
       </c>
       <c r="K94" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -5178,7 +5310,7 @@
         <v>0</v>
       </c>
       <c r="K95" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -5204,7 +5336,7 @@
         <v>0</v>
       </c>
       <c r="K96" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -5230,7 +5362,7 @@
         <v>0</v>
       </c>
       <c r="K97" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -5256,7 +5388,7 @@
         <v>0</v>
       </c>
       <c r="K98" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -5282,7 +5414,7 @@
         <v>0</v>
       </c>
       <c r="K99" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -5314,7 +5446,7 @@
         <v>0</v>
       </c>
       <c r="K100" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2.2000000000000002</v>
       </c>
       <c r="L100" t="s">
@@ -5341,15 +5473,15 @@
         <v>0</v>
       </c>
       <c r="I101" s="1">
-        <f t="shared" ref="I101:I116" si="9">IF(NOT(E101), F101*G101, F101*0)</f>
+        <f t="shared" ref="I101:I116" si="10">IF(NOT(E101), F101*G101, F101*0)</f>
         <v>0.94</v>
       </c>
       <c r="J101" s="1">
-        <f t="shared" ref="J101:J125" si="10">IF(E101, F101*G101, F101*0)</f>
+        <f t="shared" ref="J101:J125" si="11">IF(E101, F101*G101, F101*0)</f>
         <v>0</v>
       </c>
       <c r="K101" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.94</v>
       </c>
       <c r="L101" t="s">
@@ -5376,15 +5508,15 @@
         <v>0</v>
       </c>
       <c r="I102" s="1">
+        <f t="shared" si="10"/>
+        <v>2.52</v>
+      </c>
+      <c r="J102" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="K102" s="1">
         <f t="shared" si="9"/>
-        <v>2.52</v>
-      </c>
-      <c r="J102" s="1">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="K102" s="1">
-        <f t="shared" si="8"/>
         <v>2.52</v>
       </c>
       <c r="L102" t="s">
@@ -5411,15 +5543,15 @@
         <v>0</v>
       </c>
       <c r="I103" s="1">
+        <f t="shared" si="10"/>
+        <v>2.4</v>
+      </c>
+      <c r="J103" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="K103" s="1">
         <f t="shared" si="9"/>
-        <v>2.4</v>
-      </c>
-      <c r="J103" s="1">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="K103" s="1">
-        <f t="shared" si="8"/>
         <v>2.4</v>
       </c>
       <c r="L103" t="s">
@@ -5446,15 +5578,15 @@
         <v>0</v>
       </c>
       <c r="I104" s="1">
+        <f t="shared" si="10"/>
+        <v>0.94</v>
+      </c>
+      <c r="J104" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="K104" s="1">
         <f t="shared" si="9"/>
-        <v>0.94</v>
-      </c>
-      <c r="J104" s="1">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="K104" s="1">
-        <f t="shared" si="8"/>
         <v>0.94</v>
       </c>
       <c r="L104" t="s">
@@ -5481,15 +5613,15 @@
         <v>0</v>
       </c>
       <c r="I105" s="1">
+        <f t="shared" si="10"/>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="J105" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="K105" s="1">
         <f t="shared" si="9"/>
-        <v>2.4000000000000004</v>
-      </c>
-      <c r="J105" s="1">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="K105" s="1">
-        <f t="shared" si="8"/>
         <v>2.4000000000000004</v>
       </c>
       <c r="L105" t="s">
@@ -5516,15 +5648,15 @@
         <v>0</v>
       </c>
       <c r="I106" s="1">
+        <f t="shared" si="10"/>
+        <v>1.24</v>
+      </c>
+      <c r="J106" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="K106" s="1">
         <f t="shared" si="9"/>
-        <v>1.24</v>
-      </c>
-      <c r="J106" s="1">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="K106" s="1">
-        <f t="shared" si="8"/>
         <v>1.24</v>
       </c>
       <c r="L106" t="s">
@@ -5551,15 +5683,15 @@
         <v>0</v>
       </c>
       <c r="I107" s="1">
+        <f t="shared" si="10"/>
+        <v>0.7</v>
+      </c>
+      <c r="J107" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="K107" s="1">
         <f t="shared" si="9"/>
-        <v>0.7</v>
-      </c>
-      <c r="J107" s="1">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="K107" s="1">
-        <f t="shared" si="8"/>
         <v>0.7</v>
       </c>
       <c r="L107" t="s">
@@ -5586,15 +5718,15 @@
         <v>0</v>
       </c>
       <c r="I108" s="1">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="J108" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="K108" s="1">
         <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="J108" s="1">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="K108" s="1">
-        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="L108" t="s">
@@ -5621,15 +5753,15 @@
         <v>0</v>
       </c>
       <c r="I109" s="1">
+        <f t="shared" si="10"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J109" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="K109" s="1">
         <f t="shared" si="9"/>
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="J109" s="1">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="K109" s="1">
-        <f t="shared" si="8"/>
         <v>1.1000000000000001</v>
       </c>
       <c r="L109" t="s">
@@ -5656,15 +5788,15 @@
         <v>0</v>
       </c>
       <c r="I110" s="1">
+        <f t="shared" si="10"/>
+        <v>11.1</v>
+      </c>
+      <c r="J110" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="K110" s="1">
         <f t="shared" si="9"/>
-        <v>11.1</v>
-      </c>
-      <c r="J110" s="1">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="K110" s="1">
-        <f t="shared" si="8"/>
         <v>11.1</v>
       </c>
       <c r="L110" t="s">
@@ -5691,15 +5823,15 @@
         <v>0</v>
       </c>
       <c r="I111" s="1">
+        <f t="shared" si="10"/>
+        <v>9.4</v>
+      </c>
+      <c r="J111" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="K111" s="1">
         <f t="shared" si="9"/>
-        <v>9.4</v>
-      </c>
-      <c r="J111" s="1">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="K111" s="1">
-        <f t="shared" si="8"/>
         <v>9.4</v>
       </c>
       <c r="L111" t="s">
@@ -5729,15 +5861,15 @@
         <v>0</v>
       </c>
       <c r="I112" s="1">
+        <f t="shared" si="10"/>
+        <v>8.4600000000000009</v>
+      </c>
+      <c r="J112" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="K112" s="1">
         <f t="shared" si="9"/>
-        <v>8.4600000000000009</v>
-      </c>
-      <c r="J112" s="1">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="K112" s="1">
-        <f t="shared" si="8"/>
         <v>8.4600000000000009</v>
       </c>
       <c r="L112" t="s">
@@ -5767,15 +5899,15 @@
         <v>0</v>
       </c>
       <c r="I113" s="1">
+        <f t="shared" si="10"/>
+        <v>43.6</v>
+      </c>
+      <c r="J113" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="K113" s="1">
         <f t="shared" si="9"/>
-        <v>43.6</v>
-      </c>
-      <c r="J113" s="1">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="K113" s="1">
-        <f t="shared" si="8"/>
         <v>43.6</v>
       </c>
       <c r="L113" t="s">
@@ -5802,11 +5934,11 @@
         <v>0</v>
       </c>
       <c r="I114" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>11.7</v>
       </c>
       <c r="J114" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="K114" s="1">
@@ -5840,15 +5972,15 @@
         <v>0</v>
       </c>
       <c r="I115" s="1">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="J115" s="1">
+        <f t="shared" si="11"/>
+        <v>46.44</v>
+      </c>
+      <c r="K115" s="1">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="J115" s="1">
-        <f t="shared" si="10"/>
-        <v>46.44</v>
-      </c>
-      <c r="K115" s="1">
-        <f t="shared" si="8"/>
         <v>46.44</v>
       </c>
       <c r="L115" s="2" t="s">
@@ -5875,15 +6007,15 @@
         <v>0</v>
       </c>
       <c r="I116" s="1">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="J116" s="1">
+        <f t="shared" si="11"/>
+        <v>6.12</v>
+      </c>
+      <c r="K116" s="1">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="J116" s="1">
-        <f t="shared" si="10"/>
-        <v>6.12</v>
-      </c>
-      <c r="K116" s="1">
-        <f t="shared" si="8"/>
         <v>6.12</v>
       </c>
       <c r="L116" s="2" t="s">
@@ -5916,11 +6048,11 @@
         <v>69.42</v>
       </c>
       <c r="J117" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="K117" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="L117" s="2" t="s">
@@ -5945,11 +6077,11 @@
         <v>0</v>
       </c>
       <c r="I118" s="1">
-        <f t="shared" ref="I118:I125" si="11">IF(NOT(E118), F118*G118, F118*0)</f>
+        <f t="shared" ref="I118:I125" si="12">IF(NOT(E118), F118*G118, F118*0)</f>
         <v>0</v>
       </c>
       <c r="J118" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="K118" s="1">
@@ -5980,15 +6112,15 @@
         <v>0</v>
       </c>
       <c r="I119" s="1">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="J119" s="1">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="J119" s="1">
-        <f t="shared" si="10"/>
         <v>139.80000000000001</v>
       </c>
       <c r="K119" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>139.80000000000001</v>
       </c>
       <c r="L119" s="2" t="s">
@@ -6013,15 +6145,15 @@
         <v>0</v>
       </c>
       <c r="I120" s="1">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="J120" s="1">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="J120" s="1">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
       <c r="K120" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -6043,15 +6175,15 @@
         <v>0</v>
       </c>
       <c r="I121" s="1">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="J121" s="1">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="J121" s="1">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
       <c r="K121" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -6078,15 +6210,15 @@
         <v>0</v>
       </c>
       <c r="I122" s="1">
+        <f t="shared" si="12"/>
+        <v>82.22</v>
+      </c>
+      <c r="J122" s="1">
         <f t="shared" si="11"/>
-        <v>82.22</v>
-      </c>
-      <c r="J122" s="1">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K122" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>82.22</v>
       </c>
       <c r="L122" t="s">
@@ -6107,15 +6239,15 @@
         <v>0</v>
       </c>
       <c r="I123" s="1">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="J123" s="1">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="J123" s="1">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
       <c r="K123" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -6142,15 +6274,15 @@
         <v>0</v>
       </c>
       <c r="I124" s="1">
+        <f t="shared" si="12"/>
+        <v>59.99</v>
+      </c>
+      <c r="J124" s="1">
         <f t="shared" si="11"/>
-        <v>59.99</v>
-      </c>
-      <c r="J124" s="1">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K124" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>59.99</v>
       </c>
       <c r="L124" t="s">
@@ -6180,15 +6312,15 @@
         <v>0</v>
       </c>
       <c r="I125" s="1">
+        <f t="shared" si="12"/>
+        <v>79.91</v>
+      </c>
+      <c r="J125" s="1">
         <f t="shared" si="11"/>
-        <v>79.91</v>
-      </c>
-      <c r="J125" s="1">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K125" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>79.91</v>
       </c>
       <c r="L125" t="s">
@@ -6202,28 +6334,33 @@
       </c>
       <c r="J126" s="1">
         <f>SUM(J5:J125)</f>
-        <v>662.5</v>
+        <v>701.98</v>
       </c>
       <c r="K126" s="1">
         <f>SUM(K5:K125)</f>
-        <v>1949.2600000000004</v>
+        <v>1988.7400000000005</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="20" type="noConversion"/>
-  <conditionalFormatting sqref="H5:H59 H62:H125">
-    <cfRule type="expression" dxfId="9" priority="1" stopIfTrue="1">
+  <conditionalFormatting sqref="H5:H59 H62:H87 H90:H125">
+    <cfRule type="expression" dxfId="17" priority="2" stopIfTrue="1">
       <formula>$H5:$H125&gt;=$G5:$G125</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H60">
-    <cfRule type="expression" dxfId="8" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="3" stopIfTrue="1">
       <formula>$H60:$H181&gt;=$G60:$G181</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H61">
-    <cfRule type="expression" dxfId="7" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="6" stopIfTrue="1">
       <formula>$H61:$H180&gt;=$G61:$G180</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H88:H89">
+    <cfRule type="expression" dxfId="14" priority="1" stopIfTrue="1">
+      <formula>$H88:$H180&gt;=$G88:$G180</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -6244,8 +6381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F651F1D0-7A81-0546-9600-A8B0A78885C7}">
   <dimension ref="A1:K70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6394,7 +6531,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="1">
-        <v>9.3000000000000007</v>
+        <v>13.8</v>
       </c>
       <c r="F7">
         <v>5</v>
@@ -6408,11 +6545,11 @@
       </c>
       <c r="I7" s="1">
         <f t="shared" si="1"/>
-        <v>46.5</v>
+        <v>69</v>
       </c>
       <c r="J7" s="1">
         <f t="shared" si="2"/>
-        <v>46.5</v>
+        <v>69</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>145</v>
@@ -6498,7 +6635,16 @@
       <c r="B10">
         <v>1</v>
       </c>
+      <c r="C10" t="s">
+        <v>286</v>
+      </c>
       <c r="D10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1">
+        <v>7.99</v>
+      </c>
+      <c r="F10">
         <v>1</v>
       </c>
       <c r="G10">
@@ -6510,11 +6656,14 @@
       </c>
       <c r="I10" s="1">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>7.99</v>
       </c>
       <c r="J10" s="1">
         <f>(F10-G10)*E10</f>
-        <v>0</v>
+        <v>7.99</v>
+      </c>
+      <c r="K10" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -6524,7 +6673,16 @@
       <c r="B11">
         <v>1</v>
       </c>
+      <c r="C11" t="s">
+        <v>286</v>
+      </c>
       <c r="D11" t="b">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1">
+        <v>8.99</v>
+      </c>
+      <c r="F11">
         <v>1</v>
       </c>
       <c r="G11">
@@ -6536,11 +6694,14 @@
       </c>
       <c r="I11" s="1">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>8.99</v>
       </c>
       <c r="J11" s="1">
-        <f t="shared" ref="J11:J18" si="6">(F11-G11)*E11</f>
-        <v>0</v>
+        <f t="shared" ref="J11" si="6">(F11-G11)*E11</f>
+        <v>8.99</v>
+      </c>
+      <c r="K11" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -6574,7 +6735,7 @@
         <v>46.44</v>
       </c>
       <c r="J12" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="J12:J18" si="7">(F12-G12)*E12</f>
         <v>46.44</v>
       </c>
       <c r="K12" s="2" t="s">
@@ -6609,7 +6770,7 @@
         <v>6.12</v>
       </c>
       <c r="J13" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>6.12</v>
       </c>
       <c r="K13" s="2" t="s">
@@ -6643,7 +6804,7 @@
         <v>0</v>
       </c>
       <c r="J14" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K14" s="2" t="s">
@@ -6668,7 +6829,7 @@
         <v>0</v>
       </c>
       <c r="H15" s="1">
-        <f t="shared" ref="H15:H18" si="7">IF(NOT(D15), E15*F15, E15*0)</f>
+        <f t="shared" ref="H15:H18" si="8">IF(NOT(D15), E15*F15, E15*0)</f>
         <v>0</v>
       </c>
       <c r="I15" s="1">
@@ -6703,7 +6864,7 @@
         <v>0</v>
       </c>
       <c r="H16" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I16" s="1">
@@ -6711,7 +6872,7 @@
         <v>139.80000000000001</v>
       </c>
       <c r="J16" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>139.80000000000001</v>
       </c>
       <c r="K16" s="2" t="s">
@@ -6736,7 +6897,7 @@
         <v>0</v>
       </c>
       <c r="H17" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I17" s="1">
@@ -6744,7 +6905,7 @@
         <v>0</v>
       </c>
       <c r="J17" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -6766,7 +6927,7 @@
         <v>0</v>
       </c>
       <c r="H18" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I18" s="1">
@@ -6774,7 +6935,7 @@
         <v>0</v>
       </c>
       <c r="J18" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -6785,11 +6946,11 @@
       </c>
       <c r="I19" s="1">
         <f>SUM(I5:I18)</f>
-        <v>662.5</v>
+        <v>701.98</v>
       </c>
       <c r="J19" s="1">
         <f>SUM(J5:J18)</f>
-        <v>662.5</v>
+        <v>701.98</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
@@ -6803,39 +6964,39 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G12:G18">
-    <cfRule type="expression" dxfId="6" priority="37" stopIfTrue="1">
-      <formula>$H12:$H128&gt;=$G12:$G128</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G10:G11">
-    <cfRule type="expression" dxfId="5" priority="38" stopIfTrue="1">
-      <formula>$H10:$H101&gt;=$G10:$G101</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G9">
-    <cfRule type="expression" dxfId="4" priority="39" stopIfTrue="1">
-      <formula>$H9:$H92&gt;=$G9:$G92</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G8">
-    <cfRule type="expression" dxfId="3" priority="40" stopIfTrue="1">
-      <formula>$H8:$H56&gt;=$G8:$G56</formula>
+  <conditionalFormatting sqref="G5">
+    <cfRule type="expression" dxfId="13" priority="44" stopIfTrue="1">
+      <formula>$G5:$G34&gt;=$F5:$F34</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6">
-    <cfRule type="expression" dxfId="2" priority="41" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="42" stopIfTrue="1">
       <formula>$G6:$G37&gt;=$F6:$F37</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7">
-    <cfRule type="expression" dxfId="1" priority="42" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="43" stopIfTrue="1">
       <formula>$H7:$H53&gt;=$G7:$G53</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G5">
-    <cfRule type="expression" dxfId="0" priority="43" stopIfTrue="1">
-      <formula>$G5:$G34&gt;=$F5:$F34</formula>
+  <conditionalFormatting sqref="G8">
+    <cfRule type="expression" dxfId="10" priority="41" stopIfTrue="1">
+      <formula>$H8:$H56&gt;=$G8:$G56</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G9">
+    <cfRule type="expression" dxfId="9" priority="40" stopIfTrue="1">
+      <formula>$H9:$H92&gt;=$G9:$G92</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G10:G11">
+    <cfRule type="expression" dxfId="8" priority="1" stopIfTrue="1">
+      <formula>$H10:$H102&gt;=$G10:$G102</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G12:G18">
+    <cfRule type="expression" dxfId="7" priority="38" stopIfTrue="1">
+      <formula>$H12:$H128&gt;=$G12:$G128</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -6847,4 +7008,677 @@
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4686087C-B58C-7A42-AAAC-3D022FB0521D}">
+  <dimension ref="A1:K71"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="77.6640625" customWidth="1"/>
+    <col min="2" max="2" width="10.5" customWidth="1"/>
+    <col min="3" max="3" width="24.5" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" customWidth="1"/>
+    <col min="5" max="5" width="11.5" customWidth="1"/>
+    <col min="6" max="6" width="13.5" customWidth="1"/>
+    <col min="7" max="8" width="11" customWidth="1"/>
+    <col min="9" max="9" width="12.5" customWidth="1"/>
+    <col min="10" max="10" width="16.1640625" customWidth="1"/>
+    <col min="11" max="11" width="18.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>254</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>200</v>
+      </c>
+      <c r="E4" t="s">
+        <v>114</v>
+      </c>
+      <c r="F4" t="s">
+        <v>252</v>
+      </c>
+      <c r="G4" t="s">
+        <v>253</v>
+      </c>
+      <c r="H4" t="s">
+        <v>199</v>
+      </c>
+      <c r="I4" t="s">
+        <v>198</v>
+      </c>
+      <c r="J4" t="s">
+        <v>223</v>
+      </c>
+      <c r="K4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5">
+        <v>247</v>
+      </c>
+      <c r="D5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="F5">
+        <v>250</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" ref="H5:H13" si="0">IF(NOT(D5), E5*F5, E5*0)</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="1">
+        <f t="shared" ref="I5:I18" si="1">IF(D5, E5*F5, E5*0)</f>
+        <v>30</v>
+      </c>
+      <c r="J5" s="1">
+        <f t="shared" ref="J5:J9" si="2">(F5-G5)*E5</f>
+        <v>30</v>
+      </c>
+      <c r="K5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6">
+        <v>163</v>
+      </c>
+      <c r="C6" t="s">
+        <v>137</v>
+      </c>
+      <c r="D6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1">
+        <v>12.88</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
+        <f t="shared" si="1"/>
+        <v>25.76</v>
+      </c>
+      <c r="J6" s="1">
+        <f t="shared" si="2"/>
+        <v>25.76</v>
+      </c>
+      <c r="K6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>265</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>266</v>
+      </c>
+      <c r="D7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1">
+        <v>13.8</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I7" s="1">
+        <f t="shared" si="1"/>
+        <v>69</v>
+      </c>
+      <c r="J7" s="1">
+        <f t="shared" si="2"/>
+        <v>69</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>267</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="D8" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" s="3">
+        <v>66</v>
+      </c>
+      <c r="F8">
+        <v>4</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I8" s="1">
+        <f t="shared" si="1"/>
+        <v>264</v>
+      </c>
+      <c r="J8" s="1">
+        <f t="shared" si="2"/>
+        <v>264</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>274</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>279</v>
+      </c>
+      <c r="D9" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1">
+        <v>25.97</v>
+      </c>
+      <c r="F9">
+        <v>4</v>
+      </c>
+      <c r="G9">
+        <v>4</v>
+      </c>
+      <c r="H9" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I9" s="1">
+        <f t="shared" si="1"/>
+        <v>103.88</v>
+      </c>
+      <c r="J9" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K9" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>286</v>
+      </c>
+      <c r="D10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1">
+        <v>7.99</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I10" s="1">
+        <f t="shared" si="1"/>
+        <v>7.99</v>
+      </c>
+      <c r="J10" s="1">
+        <f>(F10-G10)*E10</f>
+        <v>7.99</v>
+      </c>
+      <c r="K10" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>286</v>
+      </c>
+      <c r="D11" t="b">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1">
+        <v>8.99</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I11" s="1">
+        <f t="shared" si="1"/>
+        <v>8.99</v>
+      </c>
+      <c r="J11" s="1">
+        <f t="shared" ref="J11:J19" si="3">(F11-G11)*E11</f>
+        <v>8.99</v>
+      </c>
+      <c r="K11" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>276</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>277</v>
+      </c>
+      <c r="D12" t="b">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1">
+        <v>46.44</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="1">
+        <f t="shared" si="1"/>
+        <v>46.44</v>
+      </c>
+      <c r="J12" s="1">
+        <f t="shared" si="3"/>
+        <v>46.44</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="D13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1">
+        <v>6.12</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I13" s="1">
+        <f t="shared" si="1"/>
+        <v>6.12</v>
+      </c>
+      <c r="J13" s="1">
+        <f t="shared" si="3"/>
+        <v>6.12</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>256</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>288</v>
+      </c>
+      <c r="D14" t="b">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1">
+        <v>39.950000000000003</v>
+      </c>
+      <c r="F14">
+        <v>3</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0</v>
+      </c>
+      <c r="I14" s="1">
+        <f t="shared" si="1"/>
+        <v>119.85000000000001</v>
+      </c>
+      <c r="J14" s="1">
+        <f t="shared" si="3"/>
+        <v>119.85000000000001</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>231</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>248</v>
+      </c>
+      <c r="D15" t="b">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15" s="1">
+        <f t="shared" ref="H15:H18" si="4">IF(NOT(D15), E15*F15, E15*0)</f>
+        <v>0</v>
+      </c>
+      <c r="I15" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J15" s="1">
+        <f>(F15-G15)*E15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>269</v>
+      </c>
+      <c r="B16">
+        <v>4</v>
+      </c>
+      <c r="C16" t="s">
+        <v>283</v>
+      </c>
+      <c r="D16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1">
+        <v>52.95</v>
+      </c>
+      <c r="F16">
+        <v>4</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I16" s="1">
+        <f t="shared" si="1"/>
+        <v>211.8</v>
+      </c>
+      <c r="J16" s="1">
+        <f t="shared" si="3"/>
+        <v>211.8</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>270</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>248</v>
+      </c>
+      <c r="D17" t="b">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I17" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J17" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>271</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>248</v>
+      </c>
+      <c r="D18" t="b">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I18" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J18" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>282</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="D19" t="b">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1">
+        <v>10.35</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19" s="1">
+        <f t="shared" ref="H19" si="5">IF(NOT(D19), E19*F19, E19*0)</f>
+        <v>0</v>
+      </c>
+      <c r="I19" s="1">
+        <f t="shared" ref="I19" si="6">IF(D19, E19*F19, E19*0)</f>
+        <v>10.35</v>
+      </c>
+      <c r="J19" s="1">
+        <f t="shared" si="3"/>
+        <v>10.35</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H20" s="1">
+        <f>SUM(H5:H18)</f>
+        <v>0</v>
+      </c>
+      <c r="I20" s="1">
+        <f>SUM(I5:I18)</f>
+        <v>893.82999999999993</v>
+      </c>
+      <c r="J20" s="1">
+        <f>SUM(J5:J18)</f>
+        <v>789.95</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="G5">
+    <cfRule type="expression" dxfId="6" priority="7" stopIfTrue="1">
+      <formula>$G5:$G35&gt;=$F5:$F35</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G6">
+    <cfRule type="expression" dxfId="5" priority="5" stopIfTrue="1">
+      <formula>$G6:$G38&gt;=$F6:$F38</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G7">
+    <cfRule type="expression" dxfId="4" priority="6" stopIfTrue="1">
+      <formula>$H7:$H54&gt;=$G7:$G54</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G8">
+    <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
+      <formula>$H8:$H57&gt;=$G8:$G57</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G9">
+    <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
+      <formula>$H9:$H93&gt;=$G9:$G93</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G10:G11">
+    <cfRule type="expression" dxfId="1" priority="44" stopIfTrue="1">
+      <formula>$H10:$H102&gt;=$G10:$G102</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G12:G19">
+    <cfRule type="expression" dxfId="0" priority="45" stopIfTrue="1">
+      <formula>$H12:$H129&gt;=$G12:$G129</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="K8" r:id="rId1" xr:uid="{C8EE4B32-8CD9-A74B-8028-1A42D2252BF7}"/>
+    <hyperlink ref="K7" r:id="rId2" xr:uid="{87809C0B-9BE0-1646-9431-F2DB18E2F45C}"/>
+    <hyperlink ref="K16" r:id="rId3" xr:uid="{D015C5EB-6B16-0744-8964-924D048D7799}"/>
+    <hyperlink ref="K12" r:id="rId4" xr:uid="{12807C18-4389-A048-8727-C611F66FBDB4}"/>
+    <hyperlink ref="K13" r:id="rId5" xr:uid="{83A8E58B-ACC1-BB4F-9098-CB1F1D3CF474}"/>
+    <hyperlink ref="K14" r:id="rId6" xr:uid="{87546791-3990-2846-B60F-64D77FF64AB4}"/>
+    <hyperlink ref="K19" r:id="rId7" xr:uid="{8FEB2D40-243D-EB40-9049-84074FF0142B}"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adds Manuals and STL files from mods githubs.
</commit_message>
<xml_diff>
--- a/voron_2_tall_bom.xlsx
+++ b/voron_2_tall_bom.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ppak/GitHub/Voron-2-Tall/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBE1006C-2D86-C64B-B30D-9240C60A7B76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A2FB0B-7859-BE43-8650-CA06DA24E690}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="7800" windowWidth="33600" windowHeight="21000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="generated_bom" sheetId="1" r:id="rId1"/>
@@ -7015,7 +7015,7 @@
   <dimension ref="A1:K71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7580,7 +7580,7 @@
         <v>282</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D19" t="b">
         <v>1</v>
@@ -7589,7 +7589,7 @@
         <v>10.35</v>
       </c>
       <c r="F19">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G19">
         <v>0</v>
@@ -7600,11 +7600,11 @@
       </c>
       <c r="I19" s="1">
         <f t="shared" ref="I19" si="6">IF(D19, E19*F19, E19*0)</f>
-        <v>10.35</v>
+        <v>51.75</v>
       </c>
       <c r="J19" s="1">
         <f t="shared" si="3"/>
-        <v>10.35</v>
+        <v>51.75</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>281</v>

</xml_diff>

<commit_message>
Adds Manuals and additional printed parts.
</commit_message>
<xml_diff>
--- a/voron_2_tall_bom.xlsx
+++ b/voron_2_tall_bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ppak/GitHub/Voron-2-Tall/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A2FB0B-7859-BE43-8650-CA06DA24E690}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBDDDBFB-77E2-284E-9ABB-5FB92BDE0257}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="generated_bom" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="298">
   <si>
     <t>Category</t>
   </si>
@@ -880,12 +880,6 @@
     <t>https://www.amazon.com/gp/product/B0C94YGTKX/ref=ox_sc_act_title_1?smid=A3E9XRLGZKR0KS&amp;th=1</t>
   </si>
   <si>
-    <t>https://www.amazon.com/gp/product/B0B5YJSQD3/ref=ewc_pr_img_2?smid=ATVPDKIKX0DER&amp;psc=1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rust-Oleum 372700 Acrylic Enamel 2X Spray Paint, 12 oz, Ultra Matte White </t>
-  </si>
-  <si>
     <t>24" x 48" x 1/8" Orange</t>
   </si>
   <si>
@@ -902,6 +896,39 @@
   </si>
   <si>
     <t>36" x 24" x 1/8" Orange</t>
+  </si>
+  <si>
+    <t>White Drag Chain R18 10x11 Open</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/3256805618753942.html?spm=a2g0o.order_detail.order_detail_item.4.1c4af19cX5NfXo</t>
+  </si>
+  <si>
+    <t>Replaces IGUS E2i-10-10-018-0 Chain</t>
+  </si>
+  <si>
+    <t>White Drag Chain R28 10x15 Open</t>
+  </si>
+  <si>
+    <t>Replaces IGUS E2-15-10-028-0 Chain</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/3256805618753942.html?spm=a2g0o.order_detail.order_detail_item.7.1c4af19cX5NfXo</t>
+  </si>
+  <si>
+    <t>Acrylic Sheet Orange (replaces Coroplast Sheet) - 469x469x4 mm</t>
+  </si>
+  <si>
+    <t>Door Panels</t>
+  </si>
+  <si>
+    <t>Side and Back Panels</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Krylon-K05545007-COLORmaxx-Spray-Aerosol/dp/B07LFWZ84M/ref=sr_1_1?crid=364DV301SARU2&amp;keywords=krylon%2Bspray%2Bpaint%2Bwhite&amp;qid=1704080817&amp;sprefix=krylon.%2Bwhite%2Caps%2C99&amp;sr=8-1&amp;th=1</t>
+  </si>
+  <si>
+    <t>Krylon K05545007 COLORmaxx Spray Paint and Primer for Indoor/Outdoor Use  Gloss White 12 Oz</t>
   </si>
 </sst>
 </file>
@@ -1963,8 +1990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L126"/>
   <sheetViews>
-    <sheetView topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="B115" sqref="B115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5042,7 +5069,7 @@
         <v>1</v>
       </c>
       <c r="D88" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E88" t="b">
         <v>1</v>
@@ -5069,7 +5096,7 @@
         <v>7.99</v>
       </c>
       <c r="L88" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.2">
@@ -5080,7 +5107,7 @@
         <v>1</v>
       </c>
       <c r="D89" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E89" t="b">
         <v>1</v>
@@ -5107,7 +5134,7 @@
         <v>8.99</v>
       </c>
       <c r="L89" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.2">
@@ -6343,26 +6370,6 @@
     </row>
   </sheetData>
   <phoneticPr fontId="20" type="noConversion"/>
-  <conditionalFormatting sqref="H5:H59 H62:H87 H90:H125">
-    <cfRule type="expression" dxfId="17" priority="2" stopIfTrue="1">
-      <formula>$H5:$H125&gt;=$G5:$G125</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H60">
-    <cfRule type="expression" dxfId="16" priority="3" stopIfTrue="1">
-      <formula>$H60:$H181&gt;=$G60:$G181</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H61">
-    <cfRule type="expression" dxfId="15" priority="6" stopIfTrue="1">
-      <formula>$H61:$H180&gt;=$G61:$G180</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H88:H89">
-    <cfRule type="expression" dxfId="14" priority="1" stopIfTrue="1">
-      <formula>$H88:$H180&gt;=$G88:$G180</formula>
-    </cfRule>
-  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="L29" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="L52" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
@@ -6636,7 +6643,7 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D10" t="b">
         <v>1</v>
@@ -6663,7 +6670,7 @@
         <v>7.99</v>
       </c>
       <c r="K10" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -6674,7 +6681,7 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D11" t="b">
         <v>1</v>
@@ -6701,7 +6708,7 @@
         <v>8.99</v>
       </c>
       <c r="K11" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -6964,41 +6971,6 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G5">
-    <cfRule type="expression" dxfId="13" priority="44" stopIfTrue="1">
-      <formula>$G5:$G34&gt;=$F5:$F34</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G6">
-    <cfRule type="expression" dxfId="12" priority="42" stopIfTrue="1">
-      <formula>$G6:$G37&gt;=$F6:$F37</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G7">
-    <cfRule type="expression" dxfId="11" priority="43" stopIfTrue="1">
-      <formula>$H7:$H53&gt;=$G7:$G53</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G8">
-    <cfRule type="expression" dxfId="10" priority="41" stopIfTrue="1">
-      <formula>$H8:$H56&gt;=$G8:$G56</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G9">
-    <cfRule type="expression" dxfId="9" priority="40" stopIfTrue="1">
-      <formula>$H9:$H92&gt;=$G9:$G92</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G10:G11">
-    <cfRule type="expression" dxfId="8" priority="1" stopIfTrue="1">
-      <formula>$H10:$H102&gt;=$G10:$G102</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G12:G18">
-    <cfRule type="expression" dxfId="7" priority="38" stopIfTrue="1">
-      <formula>$H12:$H128&gt;=$G12:$G128</formula>
-    </cfRule>
-  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="K8" r:id="rId1" xr:uid="{B069B4F7-3B34-1F4D-91FE-BAFC3C3AFDEB}"/>
     <hyperlink ref="K7" r:id="rId2" xr:uid="{A674AA42-7047-D742-B0B0-F79013D37D21}"/>
@@ -7012,17 +6984,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4686087C-B58C-7A42-AAAC-3D022FB0521D}">
-  <dimension ref="A1:K71"/>
+  <dimension ref="A1:K70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="77.6640625" customWidth="1"/>
+    <col min="1" max="1" width="82.5" customWidth="1"/>
     <col min="2" max="2" width="10.5" customWidth="1"/>
-    <col min="3" max="3" width="24.5" customWidth="1"/>
+    <col min="3" max="3" width="33.83203125" customWidth="1"/>
     <col min="4" max="4" width="18.6640625" customWidth="1"/>
     <col min="5" max="5" width="11.5" customWidth="1"/>
     <col min="6" max="6" width="13.5" customWidth="1"/>
@@ -7094,19 +7066,19 @@
         <v>250</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" ref="H5:H13" si="0">IF(NOT(D5), E5*F5, E5*0)</f>
         <v>0</v>
       </c>
       <c r="I5" s="1">
-        <f t="shared" ref="I5:I18" si="1">IF(D5, E5*F5, E5*0)</f>
+        <f t="shared" ref="I5:I17" si="1">IF(D5, E5*F5, E5*0)</f>
         <v>30</v>
       </c>
       <c r="J5" s="1">
         <f t="shared" ref="J5:J9" si="2">(F5-G5)*E5</f>
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="K5" t="s">
         <v>135</v>
@@ -7132,7 +7104,7 @@
         <v>2</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" si="0"/>
@@ -7144,7 +7116,7 @@
       </c>
       <c r="J6" s="1">
         <f t="shared" si="2"/>
-        <v>25.76</v>
+        <v>0</v>
       </c>
       <c r="K6" t="s">
         <v>138</v>
@@ -7170,7 +7142,7 @@
         <v>5</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H7" s="1">
         <f t="shared" si="0"/>
@@ -7182,7 +7154,7 @@
       </c>
       <c r="J7" s="1">
         <f t="shared" si="2"/>
-        <v>69</v>
+        <v>0</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>145</v>
@@ -7205,7 +7177,7 @@
         <v>4</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H8" s="1">
         <f t="shared" si="0"/>
@@ -7217,7 +7189,7 @@
       </c>
       <c r="J8" s="1">
         <f t="shared" si="2"/>
-        <v>264</v>
+        <v>0</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>268</v>
@@ -7269,7 +7241,7 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D10" t="b">
         <v>1</v>
@@ -7295,8 +7267,8 @@
         <f>(F10-G10)*E10</f>
         <v>7.99</v>
       </c>
-      <c r="K10" t="s">
-        <v>285</v>
+      <c r="K10" s="2" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -7307,7 +7279,7 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D11" t="b">
         <v>1</v>
@@ -7330,34 +7302,34 @@
         <v>8.99</v>
       </c>
       <c r="J11" s="1">
-        <f t="shared" ref="J11:J19" si="3">(F11-G11)*E11</f>
+        <f t="shared" ref="J11:J18" si="3">(F11-G11)*E11</f>
         <v>8.99</v>
       </c>
-      <c r="K11" t="s">
-        <v>287</v>
+      <c r="K11" s="2" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>276</v>
+        <v>287</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>277</v>
+        <v>289</v>
       </c>
       <c r="D12" t="b">
         <v>1</v>
       </c>
       <c r="E12" s="1">
-        <v>46.44</v>
+        <v>7.24</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H12" s="1">
         <f t="shared" si="0"/>
@@ -7365,34 +7337,37 @@
       </c>
       <c r="I12" s="1">
         <f t="shared" si="1"/>
-        <v>46.44</v>
+        <v>14.48</v>
       </c>
       <c r="J12" s="1">
         <f t="shared" si="3"/>
-        <v>46.44</v>
+        <v>0</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>217</v>
+        <v>288</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>101</v>
+        <v>290</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>291</v>
       </c>
       <c r="D13" t="b">
         <v>1</v>
       </c>
       <c r="E13" s="1">
-        <v>6.12</v>
+        <v>7.7</v>
       </c>
       <c r="F13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H13" s="1">
         <f t="shared" si="0"/>
@@ -7400,25 +7375,25 @@
       </c>
       <c r="I13" s="1">
         <f t="shared" si="1"/>
-        <v>6.12</v>
+        <v>15.4</v>
       </c>
       <c r="J13" s="1">
         <f t="shared" si="3"/>
-        <v>6.12</v>
+        <v>0</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>217</v>
+        <v>292</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>256</v>
+        <v>293</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D14" t="b">
         <v>1</v>
@@ -7449,53 +7424,56 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>231</v>
+        <v>269</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C15" t="s">
-        <v>248</v>
+        <v>281</v>
       </c>
       <c r="D15" t="b">
         <v>1</v>
       </c>
-      <c r="E15" s="1"/>
+      <c r="E15" s="1">
+        <v>52.95</v>
+      </c>
+      <c r="F15">
+        <v>4</v>
+      </c>
       <c r="G15">
         <v>0</v>
       </c>
       <c r="H15" s="1">
-        <f t="shared" ref="H15:H18" si="4">IF(NOT(D15), E15*F15, E15*0)</f>
+        <f t="shared" ref="H15:H17" si="4">IF(NOT(D15), E15*F15, E15*0)</f>
         <v>0</v>
       </c>
       <c r="I15" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>211.8</v>
       </c>
       <c r="J15" s="1">
-        <f>(F15-G15)*E15</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>211.8</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B16">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>283</v>
+        <v>294</v>
       </c>
       <c r="D16" t="b">
         <v>1</v>
       </c>
-      <c r="E16" s="1">
-        <v>52.95</v>
-      </c>
-      <c r="F16">
-        <v>4</v>
-      </c>
+      <c r="E16" s="1"/>
       <c r="G16">
         <v>0</v>
       </c>
@@ -7505,25 +7483,22 @@
       </c>
       <c r="I16" s="1">
         <f t="shared" si="1"/>
-        <v>211.8</v>
+        <v>0</v>
       </c>
       <c r="J16" s="1">
         <f t="shared" si="3"/>
-        <v>211.8</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>284</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>248</v>
+        <v>295</v>
       </c>
       <c r="D17" t="b">
         <v>1</v>
@@ -7547,137 +7522,72 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>271</v>
+        <v>297</v>
       </c>
       <c r="B18">
-        <v>2</v>
-      </c>
-      <c r="C18" t="s">
-        <v>248</v>
+        <v>8</v>
       </c>
       <c r="D18" t="b">
         <v>1</v>
       </c>
-      <c r="E18" s="1"/>
+      <c r="E18" s="1">
+        <v>6.04</v>
+      </c>
+      <c r="F18">
+        <v>8</v>
+      </c>
       <c r="G18">
         <v>0</v>
       </c>
       <c r="H18" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="H18" si="5">IF(NOT(D18), E18*F18, E18*0)</f>
         <v>0</v>
       </c>
       <c r="I18" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" ref="I18" si="6">IF(D18, E18*F18, E18*0)</f>
+        <v>48.32</v>
       </c>
       <c r="J18" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>48.32</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>282</v>
-      </c>
-      <c r="B19">
-        <v>5</v>
-      </c>
-      <c r="D19" t="b">
-        <v>1</v>
-      </c>
-      <c r="E19" s="1">
-        <v>10.35</v>
-      </c>
-      <c r="F19">
-        <v>5</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
       <c r="H19" s="1">
-        <f t="shared" ref="H19" si="5">IF(NOT(D19), E19*F19, E19*0)</f>
+        <f>SUM(H5:H17)</f>
         <v>0</v>
       </c>
       <c r="I19" s="1">
-        <f t="shared" ref="I19" si="6">IF(D19, E19*F19, E19*0)</f>
-        <v>51.75</v>
+        <f>SUM(I5:I17)</f>
+        <v>871.15000000000009</v>
       </c>
       <c r="J19" s="1">
-        <f t="shared" si="3"/>
-        <v>51.75</v>
-      </c>
-      <c r="K19" s="2" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="H20" s="1">
-        <f>SUM(H5:H18)</f>
-        <v>0</v>
-      </c>
-      <c r="I20" s="1">
-        <f>SUM(I5:I18)</f>
-        <v>893.82999999999993</v>
-      </c>
-      <c r="J20" s="1">
-        <f>SUM(J5:J18)</f>
-        <v>789.95</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
+        <f>SUM(J5:J17)</f>
+        <v>348.63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
         <v>103</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G5">
-    <cfRule type="expression" dxfId="6" priority="7" stopIfTrue="1">
-      <formula>$G5:$G35&gt;=$F5:$F35</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G6">
-    <cfRule type="expression" dxfId="5" priority="5" stopIfTrue="1">
-      <formula>$G6:$G38&gt;=$F6:$F38</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G7">
-    <cfRule type="expression" dxfId="4" priority="6" stopIfTrue="1">
-      <formula>$H7:$H54&gt;=$G7:$G54</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G8">
-    <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
-      <formula>$H8:$H57&gt;=$G8:$G57</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G9">
-    <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
-      <formula>$H9:$H93&gt;=$G9:$G93</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G10:G11">
-    <cfRule type="expression" dxfId="1" priority="44" stopIfTrue="1">
-      <formula>$H10:$H102&gt;=$G10:$G102</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G12:G19">
-    <cfRule type="expression" dxfId="0" priority="45" stopIfTrue="1">
-      <formula>$H12:$H129&gt;=$G12:$G129</formula>
-    </cfRule>
-  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="K8" r:id="rId1" xr:uid="{C8EE4B32-8CD9-A74B-8028-1A42D2252BF7}"/>
     <hyperlink ref="K7" r:id="rId2" xr:uid="{87809C0B-9BE0-1646-9431-F2DB18E2F45C}"/>
-    <hyperlink ref="K16" r:id="rId3" xr:uid="{D015C5EB-6B16-0744-8964-924D048D7799}"/>
-    <hyperlink ref="K12" r:id="rId4" xr:uid="{12807C18-4389-A048-8727-C611F66FBDB4}"/>
-    <hyperlink ref="K13" r:id="rId5" xr:uid="{83A8E58B-ACC1-BB4F-9098-CB1F1D3CF474}"/>
-    <hyperlink ref="K14" r:id="rId6" xr:uid="{87546791-3990-2846-B60F-64D77FF64AB4}"/>
-    <hyperlink ref="K19" r:id="rId7" xr:uid="{8FEB2D40-243D-EB40-9049-84074FF0142B}"/>
+    <hyperlink ref="K15" r:id="rId3" xr:uid="{D015C5EB-6B16-0744-8964-924D048D7799}"/>
+    <hyperlink ref="K14" r:id="rId4" xr:uid="{87546791-3990-2846-B60F-64D77FF64AB4}"/>
+    <hyperlink ref="K18" r:id="rId5" xr:uid="{8FEB2D40-243D-EB40-9049-84074FF0142B}"/>
+    <hyperlink ref="K10" r:id="rId6" display="https://www.amazon.com/uxcell-Temperature-Multifunctional-Insulating-Transparent/dp/B0915QTF1G/ref=sr_1_5?crid=1TE27V508QIHN&amp;keywords=ptfe%2Btubing%2B1000mm%2B4mm%2BOD%2B3mm&amp;qid=1701900349&amp;s=industrial&amp;sprefix=ptfe%2Btubing%2B1000mm%2B4mm%2Bod%2B3mm%2Cindustrial%2C75&amp;sr=1-5&amp;th=1" xr:uid="{CF2A451F-B6DF-6A4C-8220-E803525203C3}"/>
+    <hyperlink ref="K11" r:id="rId7" display="https://www.amazon.com/uxcell-Temperature-Multifunctional-Insulating-Transparent/dp/B0915BM1JD/ref=sr_1_5?crid=1TE27V508QIHN&amp;keywords=ptfe%2Btubing%2B1000mm%2B4mm%2BOD%2B3mm&amp;qid=1701900349&amp;s=industrial&amp;sprefix=ptfe%2Btubing%2B1000mm%2B4mm%2Bod%2B3mm%2Cindustrial%2C75&amp;sr=1-5&amp;th=1" xr:uid="{86B7022E-5F8A-8549-B62E-301EA489503C}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>